<commit_message>
MPTrx - removed bitrot, convert to new SIAMv4 and new frontend stuff. This version compiles but hasn't been tested yet.
</commit_message>
<xml_diff>
--- a/MPTrx/_Parcel Transportation IDP.xlsx
+++ b/MPTrx/_Parcel Transportation IDP.xlsx
@@ -1,25 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F596DAAB-F273-4A46-A0F7-38437158000E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="13800" windowHeight="5472" tabRatio="703"/>
+    <workbookView xWindow="-46188" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="703" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SIAM" sheetId="18" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="H15" authorId="0">
+    <comment ref="H15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -27,7 +38,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Rieks: </t>
         </r>
@@ -36,7 +47,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>An autoLoginAccount is an account that will automatically login when the file is uploaded. 
 There should be at most 1 such account.</t>
@@ -48,13 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="50">
-  <si>
-    <t>[Org (afko)]</t>
-  </si>
-  <si>
-    <t>orgAbbrName</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="56">
   <si>
     <t>orgFullName</t>
   </si>
@@ -62,15 +67,9 @@
     <t>Organization</t>
   </si>
   <si>
-    <t>OrgAbbrName</t>
-  </si>
-  <si>
     <t>OrgFullName</t>
   </si>
   <si>
-    <t>[PersonRegistration]</t>
-  </si>
-  <si>
     <t>personFirstName</t>
   </si>
   <si>
@@ -98,21 +97,12 @@
     <t>accPassword</t>
   </si>
   <si>
-    <t>accPerson</t>
-  </si>
-  <si>
-    <t>accOrg</t>
-  </si>
-  <si>
     <t>accAllowedRoles</t>
   </si>
   <si>
     <t>Account</t>
   </si>
   <si>
-    <t>UserID</t>
-  </si>
-  <si>
     <t>Password</t>
   </si>
   <si>
@@ -198,12 +188,51 @@
   </si>
   <si>
     <t>Role</t>
+  </si>
+  <si>
+    <t>[Organizations]</t>
+  </si>
+  <si>
+    <t>orgRef</t>
+  </si>
+  <si>
+    <t>OrgRef</t>
+  </si>
+  <si>
+    <t>[Persons]</t>
+  </si>
+  <si>
+    <t>personRef</t>
+  </si>
+  <si>
+    <t>personMiddleName</t>
+  </si>
+  <si>
+    <t>MiddleName</t>
+  </si>
+  <si>
+    <t>accActor</t>
+  </si>
+  <si>
+    <t>accParty</t>
+  </si>
+  <si>
+    <t>Actor</t>
+  </si>
+  <si>
+    <t>Party</t>
+  </si>
+  <si>
+    <t>Userid</t>
+  </si>
+  <si>
+    <t>PersonRef</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -231,13 +260,13 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -331,6 +360,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -378,7 +410,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -411,9 +443,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -446,6 +495,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -621,11 +687,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -641,13 +707,13 @@
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>2</v>
       </c>
       <c r="D1" s="7"/>
       <c r="E1" s="7"/>
@@ -657,13 +723,13 @@
     </row>
     <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
@@ -677,7 +743,7 @@
         <v>PostNL</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="3"/>
@@ -692,7 +758,7 @@
         <v>DHL</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C4"/>
       <c r="D4" s="4"/>
@@ -707,7 +773,7 @@
         <v>DPD</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="4"/>
@@ -722,7 +788,7 @@
         <v>TNT</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="4"/>
@@ -739,152 +805,160 @@
     </row>
     <row r="8" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>7</v>
+        <v>47</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
+        <v>3</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>4</v>
+      </c>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
     </row>
     <row r="9" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
+        <v>6</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>30</v>
+        <v>22</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>32</v>
+        <v>24</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>34</v>
+        <v>26</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>35</v>
+        <v>8</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C15" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>22</v>
-      </c>
       <c r="H15" s="7" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>9</v>
+        <v>52</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>3</v>
+        <v>53</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="G17" s="9" t="str">
         <f>$A17</f>
@@ -893,19 +967,19 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="G18" s="9" t="str">
         <f t="shared" ref="G18:G20" si="1">$A18</f>
@@ -914,19 +988,19 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="G19" s="9" t="str">
         <f t="shared" si="1"/>
@@ -935,19 +1009,19 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="G20" s="9" t="str">
         <f t="shared" si="1"/>

</xml_diff>